<commit_message>
First version of the Excel with phases
</commit_message>
<xml_diff>
--- a/webpage/matrix_representation.xlsx
+++ b/webpage/matrix_representation.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="985" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="IMPUTE" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="MINIMAC" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="54">
   <si>
     <t xml:space="preserve">Main stages of GUIDANCE’s workflow</t>
   </si>
@@ -37,145 +38,151 @@
     <t xml:space="preserve">phasing</t>
   </si>
   <si>
+    <t xml:space="preserve">impute</t>
+  </si>
+  <si>
+    <t xml:space="preserve">filterByInfo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">qctools</t>
+  </si>
+  <si>
+    <t xml:space="preserve">snptest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">collectSummary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mergeTwoChunks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">filterByAll</t>
+  </si>
+  <si>
+    <t xml:space="preserve">jointFilteredByAllFiles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">generateTopHits</t>
+  </si>
+  <si>
+    <t xml:space="preserve">generateQQManhattanPlots</t>
+  </si>
+  <si>
+    <t xml:space="preserve">combinePanelsComplex</t>
+  </si>
+  <si>
+    <t xml:space="preserve">combGenerateManhattanTop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phenoAnalysis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Execution’s modularity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">until_convertFromBedToBed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">until_phasing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">until_imputation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">until_qctools</t>
+  </si>
+  <si>
+    <t xml:space="preserve">until_association</t>
+  </si>
+  <si>
+    <t xml:space="preserve">until_filterByAll</t>
+  </si>
+  <si>
+    <t xml:space="preserve">until_summary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">whole_workflow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">from_phasing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">from_phasing_to_summary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">from_phasing_to_filterByAll</t>
+  </si>
+  <si>
+    <t xml:space="preserve">from_phasing_to_association</t>
+  </si>
+  <si>
+    <t xml:space="preserve">from_phasing_to_qctools</t>
+  </si>
+  <si>
+    <t xml:space="preserve">from_phasing_to_imputation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">from_imputation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">from_imputation_to_summary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">from_imputation_to_filterByAll</t>
+  </si>
+  <si>
+    <t xml:space="preserve">from_imputation_to_association</t>
+  </si>
+  <si>
+    <t xml:space="preserve">from_imputation_to_filterByInfo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">from_filterByInfo_to_qctools</t>
+  </si>
+  <si>
+    <t xml:space="preserve">from_qctools_to_association</t>
+  </si>
+  <si>
+    <t xml:space="preserve">from_association</t>
+  </si>
+  <si>
+    <t xml:space="preserve">from_association_to_filterByAll</t>
+  </si>
+  <si>
+    <t xml:space="preserve">from_association_to_summary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">from_filterByAll</t>
+  </si>
+  <si>
+    <t xml:space="preserve">from_jointFiltered_to_condensed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">from_filterByAll_to_summary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">from_manhattan_to_combine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">from_combine_to_manhattan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">from_combine_to_summary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">from_combine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">from_combineGenManTop_to_summary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">from_summary</t>
+  </si>
+  <si>
     <t xml:space="preserve">createListOfExcludedSnps</t>
   </si>
   <si>
     <t xml:space="preserve">filterHaplotypes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">impute</t>
-  </si>
-  <si>
-    <t xml:space="preserve">filterByInfo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">qctools</t>
-  </si>
-  <si>
-    <t xml:space="preserve">snptest</t>
-  </si>
-  <si>
-    <t xml:space="preserve">collectSummary</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mergeTwoChunks</t>
-  </si>
-  <si>
-    <t xml:space="preserve">filterByAll</t>
-  </si>
-  <si>
-    <t xml:space="preserve">jointFilteredByAllFiles</t>
-  </si>
-  <si>
-    <t xml:space="preserve">generateTopHits</t>
-  </si>
-  <si>
-    <t xml:space="preserve">generateQQManhattanPlots</t>
-  </si>
-  <si>
-    <t xml:space="preserve">combinePanelsComplex</t>
-  </si>
-  <si>
-    <t xml:space="preserve">combGenerateManhattanTop</t>
-  </si>
-  <si>
-    <t xml:space="preserve">phenoAnalysis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Execution’s modularity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">until_convertFromBedToBed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">until_phasing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">until_imputation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">until_qctools</t>
-  </si>
-  <si>
-    <t xml:space="preserve">until_association</t>
-  </si>
-  <si>
-    <t xml:space="preserve">until_filterByAll</t>
-  </si>
-  <si>
-    <t xml:space="preserve">until_summary</t>
-  </si>
-  <si>
-    <t xml:space="preserve">whole_workflow</t>
-  </si>
-  <si>
-    <t xml:space="preserve">from_phasing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">from_phasing_to_summary</t>
-  </si>
-  <si>
-    <t xml:space="preserve">from_phasing_to_filterByAll</t>
-  </si>
-  <si>
-    <t xml:space="preserve">from_phasing_to_qctools</t>
-  </si>
-  <si>
-    <t xml:space="preserve">from_phasing_to_association</t>
-  </si>
-  <si>
-    <t xml:space="preserve">from_phasing_to_imputation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">from_imputation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">from_imputation_to_summary</t>
-  </si>
-  <si>
-    <t xml:space="preserve">from_imputation_to_filterByAll</t>
-  </si>
-  <si>
-    <t xml:space="preserve">from_imputation_to_association</t>
-  </si>
-  <si>
-    <t xml:space="preserve">from_imputation_to_filterByInfo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">from_filterByInfo_to_qctools</t>
-  </si>
-  <si>
-    <t xml:space="preserve">from_qctools_to_association</t>
-  </si>
-  <si>
-    <t xml:space="preserve">from_association</t>
-  </si>
-  <si>
-    <t xml:space="preserve">from_association_to_filterByAll</t>
-  </si>
-  <si>
-    <t xml:space="preserve">from_association_to_summary</t>
-  </si>
-  <si>
-    <t xml:space="preserve">from_filterByAll</t>
-  </si>
-  <si>
-    <t xml:space="preserve">from_manhattan_to_combine</t>
-  </si>
-  <si>
-    <t xml:space="preserve">from_combine_to_manhattan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">from_combine_to_summary</t>
-  </si>
-  <si>
-    <t xml:space="preserve">from_combine</t>
-  </si>
-  <si>
-    <t xml:space="preserve">from_combineGenManTop_to_summary</t>
-  </si>
-  <si>
-    <t xml:space="preserve">from_summary</t>
   </si>
 </sst>
 </file>
@@ -255,7 +262,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -277,6 +284,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -357,10 +368,669 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:X80"/>
+  <dimension ref="1:82"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="3.88775510204082"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="33.6938775510204"/>
+    <col collapsed="false" hidden="false" max="22" min="3" style="0" width="3.88775510204082"/>
+    <col collapsed="false" hidden="false" max="1025" min="23" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="true" ht="21.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="2"/>
+      <c r="U1" s="2"/>
+      <c r="V1" s="2"/>
+      <c r="AMI1" s="0"/>
+      <c r="AMJ1" s="0"/>
+    </row>
+    <row r="2" customFormat="false" ht="180" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="T2" s="3"/>
+      <c r="U2" s="3"/>
+      <c r="V2" s="3"/>
+    </row>
+    <row r="3" customFormat="false" ht="3.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+    </row>
+    <row r="5" customFormat="false" ht="3.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="4"/>
+    </row>
+    <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="4"/>
+      <c r="B6" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+    </row>
+    <row r="7" customFormat="false" ht="3.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="4"/>
+    </row>
+    <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="4"/>
+      <c r="B8" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+    </row>
+    <row r="9" customFormat="false" ht="3.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="4"/>
+    </row>
+    <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="4"/>
+      <c r="B10" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+    </row>
+    <row r="11" customFormat="false" ht="3.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="4"/>
+    </row>
+    <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="4"/>
+      <c r="B12" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+    </row>
+    <row r="13" customFormat="false" ht="3.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="4"/>
+    </row>
+    <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="4"/>
+      <c r="B14" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="5"/>
+      <c r="L14" s="5"/>
+      <c r="M14" s="5"/>
+    </row>
+    <row r="15" customFormat="false" ht="3.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="4"/>
+    </row>
+    <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="4"/>
+      <c r="B16" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="5"/>
+      <c r="L16" s="5"/>
+      <c r="M16" s="5"/>
+      <c r="N16" s="5"/>
+      <c r="O16" s="5"/>
+      <c r="P16" s="5"/>
+      <c r="Q16" s="5"/>
+      <c r="R16" s="5"/>
+    </row>
+    <row r="17" customFormat="false" ht="3.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="4"/>
+    </row>
+    <row r="18" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="4"/>
+      <c r="B18" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="5"/>
+      <c r="K18" s="5"/>
+      <c r="L18" s="5"/>
+      <c r="M18" s="5"/>
+      <c r="N18" s="5"/>
+      <c r="O18" s="5"/>
+      <c r="P18" s="5"/>
+      <c r="Q18" s="5"/>
+      <c r="R18" s="5"/>
+      <c r="S18" s="5"/>
+    </row>
+    <row r="19" customFormat="false" ht="3.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="4"/>
+    </row>
+    <row r="20" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="4"/>
+      <c r="B20" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
+      <c r="I20" s="5"/>
+      <c r="J20" s="5"/>
+      <c r="K20" s="5"/>
+      <c r="L20" s="5"/>
+      <c r="M20" s="5"/>
+      <c r="N20" s="5"/>
+      <c r="O20" s="5"/>
+      <c r="P20" s="5"/>
+      <c r="Q20" s="5"/>
+      <c r="R20" s="5"/>
+      <c r="S20" s="5"/>
+    </row>
+    <row r="21" customFormat="false" ht="3.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A21" s="4"/>
+    </row>
+    <row r="22" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="4"/>
+      <c r="B22" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="5"/>
+      <c r="J22" s="5"/>
+      <c r="K22" s="5"/>
+      <c r="L22" s="5"/>
+      <c r="M22" s="5"/>
+      <c r="N22" s="5"/>
+      <c r="O22" s="5"/>
+      <c r="P22" s="5"/>
+      <c r="Q22" s="5"/>
+      <c r="R22" s="5"/>
+    </row>
+    <row r="23" customFormat="false" ht="3.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A23" s="4"/>
+    </row>
+    <row r="24" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A24" s="4"/>
+      <c r="B24" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
+      <c r="I24" s="5"/>
+      <c r="J24" s="5"/>
+      <c r="K24" s="5"/>
+      <c r="L24" s="5"/>
+      <c r="M24" s="5"/>
+    </row>
+    <row r="25" customFormat="false" ht="3.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A25" s="4"/>
+    </row>
+    <row r="26" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A26" s="4"/>
+      <c r="B26" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="G26" s="5"/>
+      <c r="H26" s="5"/>
+      <c r="I26" s="5"/>
+      <c r="J26" s="5"/>
+    </row>
+    <row r="27" customFormat="false" ht="3.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A27" s="4"/>
+    </row>
+    <row r="28" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A28" s="4"/>
+      <c r="B28" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="G28" s="5"/>
+      <c r="H28" s="5"/>
+      <c r="I28" s="5"/>
+    </row>
+    <row r="29" customFormat="false" ht="3.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A29" s="4"/>
+    </row>
+    <row r="30" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A30" s="4"/>
+      <c r="B30" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="G30" s="5"/>
+    </row>
+    <row r="31" customFormat="false" ht="3.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A31" s="4"/>
+    </row>
+    <row r="32" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A32" s="4"/>
+      <c r="B32" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="H32" s="5"/>
+      <c r="I32" s="5"/>
+      <c r="J32" s="5"/>
+      <c r="K32" s="5"/>
+      <c r="L32" s="5"/>
+      <c r="M32" s="5"/>
+      <c r="N32" s="5"/>
+      <c r="O32" s="5"/>
+      <c r="P32" s="5"/>
+      <c r="Q32" s="5"/>
+      <c r="R32" s="5"/>
+      <c r="S32" s="5"/>
+    </row>
+    <row r="33" customFormat="false" ht="3.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A33" s="4"/>
+    </row>
+    <row r="34" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A34" s="4"/>
+      <c r="B34" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="H34" s="5"/>
+      <c r="I34" s="5"/>
+      <c r="J34" s="5"/>
+      <c r="K34" s="5"/>
+      <c r="L34" s="5"/>
+      <c r="M34" s="5"/>
+      <c r="N34" s="5"/>
+      <c r="O34" s="5"/>
+      <c r="P34" s="5"/>
+      <c r="Q34" s="5"/>
+      <c r="R34" s="6"/>
+      <c r="S34" s="6"/>
+    </row>
+    <row r="35" customFormat="false" ht="3.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A35" s="4"/>
+    </row>
+    <row r="36" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A36" s="4"/>
+      <c r="B36" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="H36" s="5"/>
+      <c r="I36" s="5"/>
+      <c r="J36" s="5"/>
+      <c r="K36" s="5"/>
+      <c r="L36" s="5"/>
+      <c r="M36" s="5"/>
+      <c r="N36" s="6"/>
+      <c r="O36" s="6"/>
+      <c r="P36" s="6"/>
+      <c r="Q36" s="6"/>
+    </row>
+    <row r="37" customFormat="false" ht="3.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A37" s="4"/>
+    </row>
+    <row r="38" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A38" s="4"/>
+      <c r="B38" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="H38" s="5"/>
+      <c r="I38" s="5"/>
+      <c r="J38" s="5"/>
+    </row>
+    <row r="39" customFormat="false" ht="3.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A39" s="4"/>
+    </row>
+    <row r="40" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A40" s="4"/>
+      <c r="B40" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="H40" s="5"/>
+    </row>
+    <row r="41" customFormat="false" ht="3.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A41" s="4"/>
+    </row>
+    <row r="42" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A42" s="4"/>
+      <c r="B42" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="I42" s="5"/>
+    </row>
+    <row r="43" customFormat="false" ht="3.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A43" s="4"/>
+    </row>
+    <row r="44" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A44" s="4"/>
+      <c r="B44" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="J44" s="5"/>
+    </row>
+    <row r="45" customFormat="false" ht="3.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A45" s="4"/>
+    </row>
+    <row r="46" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A46" s="4"/>
+      <c r="B46" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="K46" s="5"/>
+      <c r="L46" s="5"/>
+      <c r="M46" s="5"/>
+      <c r="N46" s="5"/>
+      <c r="O46" s="5"/>
+      <c r="P46" s="5"/>
+      <c r="Q46" s="5"/>
+      <c r="R46" s="5"/>
+      <c r="S46" s="5"/>
+    </row>
+    <row r="47" customFormat="false" ht="3.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A47" s="4"/>
+    </row>
+    <row r="48" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A48" s="4"/>
+      <c r="B48" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="K48" s="5"/>
+      <c r="L48" s="5"/>
+      <c r="M48" s="5"/>
+    </row>
+    <row r="49" customFormat="false" ht="3.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A49" s="4"/>
+    </row>
+    <row r="50" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A50" s="4"/>
+      <c r="B50" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="K50" s="5"/>
+      <c r="L50" s="5"/>
+      <c r="M50" s="5"/>
+      <c r="N50" s="5"/>
+      <c r="O50" s="5"/>
+      <c r="P50" s="5"/>
+      <c r="Q50" s="5"/>
+      <c r="R50" s="5"/>
+    </row>
+    <row r="51" customFormat="false" ht="3.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A51" s="4"/>
+    </row>
+    <row r="52" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A52" s="4"/>
+      <c r="B52" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="N52" s="5"/>
+      <c r="O52" s="5"/>
+      <c r="P52" s="5"/>
+      <c r="Q52" s="5"/>
+      <c r="R52" s="5"/>
+      <c r="S52" s="5"/>
+    </row>
+    <row r="53" customFormat="false" ht="3.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A53" s="4"/>
+      <c r="M53" s="6"/>
+      <c r="N53" s="6"/>
+      <c r="O53" s="6"/>
+      <c r="P53" s="6"/>
+      <c r="Q53" s="6"/>
+      <c r="R53" s="6"/>
+      <c r="S53" s="6"/>
+      <c r="T53" s="6"/>
+    </row>
+    <row r="54" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A54" s="4"/>
+      <c r="B54" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="M54" s="6"/>
+      <c r="N54" s="6"/>
+      <c r="O54" s="5"/>
+      <c r="P54" s="6"/>
+      <c r="Q54" s="6"/>
+      <c r="R54" s="6"/>
+      <c r="S54" s="6"/>
+      <c r="T54" s="6"/>
+    </row>
+    <row r="55" customFormat="false" ht="3.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A55" s="4"/>
+      <c r="M55" s="6"/>
+      <c r="N55" s="6"/>
+      <c r="O55" s="6"/>
+      <c r="P55" s="6"/>
+      <c r="Q55" s="6"/>
+      <c r="R55" s="6"/>
+      <c r="S55" s="6"/>
+      <c r="T55" s="6"/>
+    </row>
+    <row r="56" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A56" s="4"/>
+      <c r="B56" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="M56" s="6"/>
+      <c r="N56" s="5"/>
+      <c r="O56" s="5"/>
+      <c r="P56" s="5"/>
+      <c r="Q56" s="5"/>
+      <c r="R56" s="5"/>
+      <c r="S56" s="6"/>
+      <c r="T56" s="6"/>
+    </row>
+    <row r="57" customFormat="false" ht="3.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A57" s="4"/>
+      <c r="M57" s="6"/>
+      <c r="N57" s="6"/>
+      <c r="O57" s="6"/>
+      <c r="P57" s="6"/>
+      <c r="Q57" s="6"/>
+      <c r="R57" s="6"/>
+      <c r="S57" s="6"/>
+      <c r="T57" s="6"/>
+    </row>
+    <row r="58" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A58" s="4"/>
+      <c r="B58" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="M58" s="6"/>
+      <c r="N58" s="6"/>
+      <c r="O58" s="6"/>
+      <c r="P58" s="5"/>
+      <c r="Q58" s="6"/>
+      <c r="R58" s="6"/>
+      <c r="S58" s="6"/>
+      <c r="T58" s="6"/>
+    </row>
+    <row r="59" customFormat="false" ht="3.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A59" s="4"/>
+    </row>
+    <row r="60" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A60" s="4"/>
+      <c r="B60" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q60" s="5"/>
+    </row>
+    <row r="61" customFormat="false" ht="3.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A61" s="4"/>
+    </row>
+    <row r="62" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A62" s="4"/>
+      <c r="B62" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q62" s="5"/>
+      <c r="R62" s="5"/>
+    </row>
+    <row r="63" customFormat="false" ht="3.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A63" s="4"/>
+    </row>
+    <row r="64" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A64" s="4"/>
+      <c r="B64" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q64" s="5"/>
+      <c r="R64" s="5"/>
+      <c r="S64" s="5"/>
+    </row>
+    <row r="65" customFormat="false" ht="3.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A65" s="4"/>
+    </row>
+    <row r="66" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A66" s="4"/>
+      <c r="B66" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="R66" s="5"/>
+    </row>
+    <row r="67" customFormat="false" ht="3.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A67" s="4"/>
+    </row>
+    <row r="68" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A68" s="4"/>
+      <c r="B68" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="S68" s="5"/>
+    </row>
+    <row r="69" customFormat="false" ht="3.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="70" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="71" customFormat="false" ht="3.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="72" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="73" customFormat="false" ht="3.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="74" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="75" customFormat="false" ht="3.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="76" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="77" customFormat="false" ht="3.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="78" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="79" customFormat="false" ht="3.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="80" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="81" customFormat="false" ht="3.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="82" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C1:V1"/>
+    <mergeCell ref="A4:A68"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="8" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:X82"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="V7" activeCellId="0" sqref="V7"/>
+      <selection pane="topLeft" activeCell="O27" activeCellId="0" sqref="O27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -397,7 +1067,7 @@
       <c r="W1" s="2"/>
       <c r="X1" s="2"/>
     </row>
-    <row r="2" customFormat="false" ht="129.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="180" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C2" s="3" t="s">
         <v>1</v>
       </c>
@@ -411,49 +1081,49 @@
         <v>4</v>
       </c>
       <c r="G2" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="I2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="J2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="K2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="L2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="M2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="N2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="O2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="P2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="O2" s="3" t="s">
+      <c r="Q2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="P2" s="3" t="s">
+      <c r="R2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="Q2" s="3" t="s">
+      <c r="S2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="R2" s="3" t="s">
+      <c r="T2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="S2" s="3" t="s">
+      <c r="U2" s="3" t="s">
         <v>17</v>
-      </c>
-      <c r="T2" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="U2" s="3" t="s">
-        <v>19</v>
       </c>
       <c r="V2" s="3"/>
       <c r="W2" s="3"/>
@@ -462,10 +1132,10 @@
     <row r="3" customFormat="false" ht="3.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
@@ -476,12 +1146,14 @@
     <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="4"/>
       <c r="B6" s="0" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
     </row>
     <row r="7" customFormat="false" ht="3.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="4"/>
@@ -489,12 +1161,14 @@
     <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="4"/>
       <c r="B8" s="0" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
       <c r="I8" s="5"/>
     </row>
     <row r="9" customFormat="false" ht="3.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -503,12 +1177,14 @@
     <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="4"/>
       <c r="B10" s="0" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
       <c r="I10" s="5"/>
       <c r="J10" s="5"/>
       <c r="K10" s="5"/>
@@ -519,12 +1195,14 @@
     <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="4"/>
       <c r="B12" s="0" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
       <c r="I12" s="5"/>
       <c r="J12" s="5"/>
       <c r="K12" s="5"/>
@@ -536,12 +1214,14 @@
     <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="4"/>
       <c r="B14" s="0" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
       <c r="I14" s="5"/>
       <c r="J14" s="5"/>
       <c r="K14" s="5"/>
@@ -556,12 +1236,14 @@
     <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="4"/>
       <c r="B16" s="0" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
       <c r="I16" s="5"/>
       <c r="J16" s="5"/>
       <c r="K16" s="5"/>
@@ -581,12 +1263,14 @@
     <row r="18" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="4"/>
       <c r="B18" s="0" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
       <c r="I18" s="5"/>
       <c r="J18" s="5"/>
       <c r="K18" s="5"/>
@@ -607,8 +1291,21 @@
     <row r="20" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="4"/>
       <c r="B20" s="0" t="s">
-        <v>29</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="I20" s="5"/>
+      <c r="J20" s="5"/>
+      <c r="K20" s="5"/>
+      <c r="L20" s="5"/>
+      <c r="M20" s="5"/>
+      <c r="N20" s="5"/>
+      <c r="O20" s="5"/>
+      <c r="P20" s="5"/>
+      <c r="Q20" s="5"/>
+      <c r="R20" s="5"/>
+      <c r="S20" s="5"/>
+      <c r="T20" s="5"/>
+      <c r="U20" s="5"/>
     </row>
     <row r="21" customFormat="false" ht="3.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="4"/>
@@ -616,8 +1313,20 @@
     <row r="22" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="4"/>
       <c r="B22" s="0" t="s">
-        <v>30</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="I22" s="5"/>
+      <c r="J22" s="5"/>
+      <c r="K22" s="5"/>
+      <c r="L22" s="5"/>
+      <c r="M22" s="5"/>
+      <c r="N22" s="5"/>
+      <c r="O22" s="5"/>
+      <c r="P22" s="5"/>
+      <c r="Q22" s="5"/>
+      <c r="R22" s="5"/>
+      <c r="S22" s="5"/>
+      <c r="T22" s="5"/>
     </row>
     <row r="23" customFormat="false" ht="3.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="4"/>
@@ -625,8 +1334,15 @@
     <row r="24" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="4"/>
       <c r="B24" s="0" t="s">
-        <v>31</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="I24" s="5"/>
+      <c r="J24" s="5"/>
+      <c r="K24" s="5"/>
+      <c r="L24" s="5"/>
+      <c r="M24" s="5"/>
+      <c r="N24" s="5"/>
+      <c r="O24" s="5"/>
     </row>
     <row r="25" customFormat="false" ht="3.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="4"/>
@@ -634,8 +1350,12 @@
     <row r="26" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="4"/>
       <c r="B26" s="0" t="s">
-        <v>32</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="I26" s="5"/>
+      <c r="J26" s="5"/>
+      <c r="K26" s="5"/>
+      <c r="L26" s="5"/>
     </row>
     <row r="27" customFormat="false" ht="3.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="4"/>
@@ -643,8 +1363,11 @@
     <row r="28" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="4"/>
       <c r="B28" s="0" t="s">
-        <v>33</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="I28" s="5"/>
+      <c r="J28" s="5"/>
+      <c r="K28" s="5"/>
     </row>
     <row r="29" customFormat="false" ht="3.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="4"/>
@@ -654,6 +1377,7 @@
       <c r="B30" s="0" t="s">
         <v>32</v>
       </c>
+      <c r="I30" s="5"/>
     </row>
     <row r="31" customFormat="false" ht="3.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="4"/>
@@ -661,8 +1385,20 @@
     <row r="32" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="4"/>
       <c r="B32" s="0" t="s">
-        <v>34</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="J32" s="5"/>
+      <c r="K32" s="5"/>
+      <c r="L32" s="5"/>
+      <c r="M32" s="5"/>
+      <c r="N32" s="5"/>
+      <c r="O32" s="5"/>
+      <c r="P32" s="5"/>
+      <c r="Q32" s="5"/>
+      <c r="R32" s="5"/>
+      <c r="S32" s="5"/>
+      <c r="T32" s="5"/>
+      <c r="U32" s="5"/>
     </row>
     <row r="33" customFormat="false" ht="3.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="4"/>
@@ -670,8 +1406,20 @@
     <row r="34" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="4"/>
       <c r="B34" s="0" t="s">
-        <v>35</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="J34" s="5"/>
+      <c r="K34" s="5"/>
+      <c r="L34" s="5"/>
+      <c r="M34" s="5"/>
+      <c r="N34" s="5"/>
+      <c r="O34" s="5"/>
+      <c r="P34" s="5"/>
+      <c r="Q34" s="5"/>
+      <c r="R34" s="5"/>
+      <c r="S34" s="5"/>
+      <c r="T34" s="6"/>
+      <c r="U34" s="6"/>
     </row>
     <row r="35" customFormat="false" ht="3.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="4"/>
@@ -679,8 +1427,18 @@
     <row r="36" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="4"/>
       <c r="B36" s="0" t="s">
-        <v>36</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="J36" s="5"/>
+      <c r="K36" s="5"/>
+      <c r="L36" s="5"/>
+      <c r="M36" s="5"/>
+      <c r="N36" s="5"/>
+      <c r="O36" s="5"/>
+      <c r="P36" s="6"/>
+      <c r="Q36" s="6"/>
+      <c r="R36" s="6"/>
+      <c r="S36" s="6"/>
     </row>
     <row r="37" customFormat="false" ht="3.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="4"/>
@@ -688,8 +1446,11 @@
     <row r="38" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="4"/>
       <c r="B38" s="0" t="s">
-        <v>37</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="J38" s="5"/>
+      <c r="K38" s="5"/>
+      <c r="L38" s="5"/>
     </row>
     <row r="39" customFormat="false" ht="3.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="4"/>
@@ -697,8 +1458,9 @@
     <row r="40" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="4"/>
       <c r="B40" s="0" t="s">
-        <v>38</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="J40" s="5"/>
     </row>
     <row r="41" customFormat="false" ht="3.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="4"/>
@@ -706,8 +1468,9 @@
     <row r="42" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="4"/>
       <c r="B42" s="0" t="s">
-        <v>39</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="K42" s="5"/>
     </row>
     <row r="43" customFormat="false" ht="3.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="4"/>
@@ -715,8 +1478,9 @@
     <row r="44" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="4"/>
       <c r="B44" s="0" t="s">
-        <v>40</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="L44" s="5"/>
     </row>
     <row r="45" customFormat="false" ht="3.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="4"/>
@@ -724,8 +1488,17 @@
     <row r="46" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="4"/>
       <c r="B46" s="0" t="s">
-        <v>41</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="M46" s="5"/>
+      <c r="N46" s="5"/>
+      <c r="O46" s="5"/>
+      <c r="P46" s="5"/>
+      <c r="Q46" s="5"/>
+      <c r="R46" s="5"/>
+      <c r="S46" s="5"/>
+      <c r="T46" s="5"/>
+      <c r="U46" s="5"/>
     </row>
     <row r="47" customFormat="false" ht="3.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="4"/>
@@ -733,8 +1506,11 @@
     <row r="48" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="4"/>
       <c r="B48" s="0" t="s">
-        <v>42</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="M48" s="5"/>
+      <c r="N48" s="5"/>
+      <c r="O48" s="5"/>
     </row>
     <row r="49" customFormat="false" ht="3.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="4"/>
@@ -742,8 +1518,16 @@
     <row r="50" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="4"/>
       <c r="B50" s="0" t="s">
-        <v>43</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="M50" s="5"/>
+      <c r="N50" s="5"/>
+      <c r="O50" s="5"/>
+      <c r="P50" s="5"/>
+      <c r="Q50" s="5"/>
+      <c r="R50" s="5"/>
+      <c r="S50" s="5"/>
+      <c r="T50" s="5"/>
     </row>
     <row r="51" customFormat="false" ht="3.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="4"/>
@@ -751,35 +1535,89 @@
     <row r="52" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="4"/>
       <c r="B52" s="0" t="s">
-        <v>44</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="P52" s="5"/>
+      <c r="Q52" s="5"/>
+      <c r="R52" s="5"/>
+      <c r="S52" s="5"/>
+      <c r="T52" s="5"/>
+      <c r="U52" s="5"/>
     </row>
     <row r="53" customFormat="false" ht="3.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="4"/>
+      <c r="O53" s="6"/>
+      <c r="P53" s="6"/>
+      <c r="Q53" s="6"/>
+      <c r="R53" s="6"/>
+      <c r="S53" s="6"/>
+      <c r="T53" s="6"/>
+      <c r="U53" s="6"/>
+      <c r="V53" s="6"/>
     </row>
     <row r="54" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="4"/>
       <c r="B54" s="0" t="s">
-        <v>45</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="O54" s="6"/>
+      <c r="P54" s="6"/>
+      <c r="Q54" s="5"/>
+      <c r="R54" s="6"/>
+      <c r="S54" s="6"/>
+      <c r="T54" s="6"/>
+      <c r="U54" s="6"/>
+      <c r="V54" s="6"/>
     </row>
     <row r="55" customFormat="false" ht="3.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="4"/>
+      <c r="O55" s="6"/>
+      <c r="P55" s="6"/>
+      <c r="Q55" s="6"/>
+      <c r="R55" s="6"/>
+      <c r="S55" s="6"/>
+      <c r="T55" s="6"/>
+      <c r="U55" s="6"/>
+      <c r="V55" s="6"/>
     </row>
     <row r="56" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="4"/>
       <c r="B56" s="0" t="s">
-        <v>46</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="O56" s="6"/>
+      <c r="P56" s="5"/>
+      <c r="Q56" s="5"/>
+      <c r="R56" s="5"/>
+      <c r="S56" s="5"/>
+      <c r="T56" s="5"/>
+      <c r="U56" s="6"/>
+      <c r="V56" s="6"/>
     </row>
     <row r="57" customFormat="false" ht="3.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="4"/>
+      <c r="O57" s="6"/>
+      <c r="P57" s="6"/>
+      <c r="Q57" s="6"/>
+      <c r="R57" s="6"/>
+      <c r="S57" s="6"/>
+      <c r="T57" s="6"/>
+      <c r="U57" s="6"/>
+      <c r="V57" s="6"/>
     </row>
     <row r="58" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="4"/>
       <c r="B58" s="0" t="s">
-        <v>47</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="O58" s="6"/>
+      <c r="P58" s="6"/>
+      <c r="Q58" s="6"/>
+      <c r="R58" s="5"/>
+      <c r="S58" s="6"/>
+      <c r="T58" s="6"/>
+      <c r="U58" s="6"/>
+      <c r="V58" s="6"/>
     </row>
     <row r="59" customFormat="false" ht="3.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="4"/>
@@ -787,8 +1625,9 @@
     <row r="60" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="4"/>
       <c r="B60" s="0" t="s">
-        <v>48</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="S60" s="5"/>
     </row>
     <row r="61" customFormat="false" ht="3.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="4"/>
@@ -796,8 +1635,10 @@
     <row r="62" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="4"/>
       <c r="B62" s="0" t="s">
-        <v>49</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="S62" s="5"/>
+      <c r="T62" s="5"/>
     </row>
     <row r="63" customFormat="false" ht="3.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="4"/>
@@ -805,8 +1646,11 @@
     <row r="64" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="4"/>
       <c r="B64" s="0" t="s">
-        <v>50</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="S64" s="5"/>
+      <c r="T64" s="5"/>
+      <c r="U64" s="5"/>
     </row>
     <row r="65" customFormat="false" ht="3.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="4"/>
@@ -814,11 +1658,20 @@
     <row r="66" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="4"/>
       <c r="B66" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="T66" s="5"/>
+    </row>
+    <row r="67" customFormat="false" ht="3.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A67" s="4"/>
+    </row>
+    <row r="68" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A68" s="4"/>
+      <c r="B68" s="0" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="67" customFormat="false" ht="3.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="68" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+      <c r="U68" s="5"/>
+    </row>
     <row r="69" customFormat="false" ht="3.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="70" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="71" customFormat="false" ht="3.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -831,14 +1684,16 @@
     <row r="78" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="79" customFormat="false" ht="3.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="80" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="81" customFormat="false" ht="3.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="82" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="C1:X1"/>
-    <mergeCell ref="A4:A66"/>
+    <mergeCell ref="A4:A68"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="8" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="8" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>

</xml_diff>

<commit_message>
Config files, stages and first configuration file parameters version
</commit_message>
<xml_diff>
--- a/webpage/matrix_representation.xlsx
+++ b/webpage/matrix_representation.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="985" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="IMPUTE" sheetId="1" state="visible" r:id="rId2"/>
@@ -146,19 +146,19 @@
     <t xml:space="preserve">from_association</t>
   </si>
   <si>
+    <t xml:space="preserve">from_association_to_summary</t>
+  </si>
+  <si>
     <t xml:space="preserve">from_association_to_filterByAll</t>
   </si>
   <si>
-    <t xml:space="preserve">from_association_to_summary</t>
-  </si>
-  <si>
     <t xml:space="preserve">from_filterByAll</t>
   </si>
   <si>
+    <t xml:space="preserve">from_filterByAll_to_summary</t>
+  </si>
+  <si>
     <t xml:space="preserve">from_jointFiltered_to_condensed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">from_filterByAll_to_summary</t>
   </si>
   <si>
     <t xml:space="preserve">from_manhattan_to_combine</t>
@@ -197,6 +197,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -262,7 +263,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -271,7 +272,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -279,15 +280,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="90" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -370,16 +367,16 @@
   </sheetPr>
   <dimension ref="1:82"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="W56" activeCellId="0" sqref="W56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="3.88775510204082"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="33.6938775510204"/>
-    <col collapsed="false" hidden="false" max="22" min="3" style="0" width="3.88775510204082"/>
-    <col collapsed="false" hidden="false" max="1025" min="23" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="3.78061224489796"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="33.3418367346939"/>
+    <col collapsed="false" hidden="false" max="22" min="3" style="0" width="3.78061224489796"/>
+    <col collapsed="false" hidden="false" max="1025" min="23" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="21.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -739,8 +736,6 @@
       <c r="O34" s="5"/>
       <c r="P34" s="5"/>
       <c r="Q34" s="5"/>
-      <c r="R34" s="6"/>
-      <c r="S34" s="6"/>
     </row>
     <row r="35" customFormat="false" ht="3.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="4"/>
@@ -756,10 +751,6 @@
       <c r="K36" s="5"/>
       <c r="L36" s="5"/>
       <c r="M36" s="5"/>
-      <c r="N36" s="6"/>
-      <c r="O36" s="6"/>
-      <c r="P36" s="6"/>
-      <c r="Q36" s="6"/>
     </row>
     <row r="37" customFormat="false" ht="3.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="4"/>
@@ -832,6 +823,11 @@
       <c r="K48" s="5"/>
       <c r="L48" s="5"/>
       <c r="M48" s="5"/>
+      <c r="N48" s="5"/>
+      <c r="O48" s="5"/>
+      <c r="P48" s="5"/>
+      <c r="Q48" s="5"/>
+      <c r="R48" s="5"/>
     </row>
     <row r="49" customFormat="false" ht="3.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="4"/>
@@ -844,11 +840,6 @@
       <c r="K50" s="5"/>
       <c r="L50" s="5"/>
       <c r="M50" s="5"/>
-      <c r="N50" s="5"/>
-      <c r="O50" s="5"/>
-      <c r="P50" s="5"/>
-      <c r="Q50" s="5"/>
-      <c r="R50" s="5"/>
     </row>
     <row r="51" customFormat="false" ht="3.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="4"/>
@@ -867,78 +858,37 @@
     </row>
     <row r="53" customFormat="false" ht="3.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="4"/>
-      <c r="M53" s="6"/>
-      <c r="N53" s="6"/>
-      <c r="O53" s="6"/>
-      <c r="P53" s="6"/>
-      <c r="Q53" s="6"/>
-      <c r="R53" s="6"/>
-      <c r="S53" s="6"/>
-      <c r="T53" s="6"/>
     </row>
     <row r="54" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="4"/>
       <c r="B54" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="M54" s="6"/>
-      <c r="N54" s="6"/>
+      <c r="N54" s="5"/>
       <c r="O54" s="5"/>
-      <c r="P54" s="6"/>
-      <c r="Q54" s="6"/>
-      <c r="R54" s="6"/>
-      <c r="S54" s="6"/>
-      <c r="T54" s="6"/>
+      <c r="P54" s="5"/>
+      <c r="Q54" s="5"/>
+      <c r="R54" s="5"/>
     </row>
     <row r="55" customFormat="false" ht="3.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="4"/>
-      <c r="M55" s="6"/>
-      <c r="N55" s="6"/>
-      <c r="O55" s="6"/>
-      <c r="P55" s="6"/>
-      <c r="Q55" s="6"/>
-      <c r="R55" s="6"/>
-      <c r="S55" s="6"/>
-      <c r="T55" s="6"/>
     </row>
     <row r="56" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="4"/>
       <c r="B56" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="M56" s="6"/>
-      <c r="N56" s="5"/>
       <c r="O56" s="5"/>
-      <c r="P56" s="5"/>
-      <c r="Q56" s="5"/>
-      <c r="R56" s="5"/>
-      <c r="S56" s="6"/>
-      <c r="T56" s="6"/>
     </row>
     <row r="57" customFormat="false" ht="3.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="4"/>
-      <c r="M57" s="6"/>
-      <c r="N57" s="6"/>
-      <c r="O57" s="6"/>
-      <c r="P57" s="6"/>
-      <c r="Q57" s="6"/>
-      <c r="R57" s="6"/>
-      <c r="S57" s="6"/>
-      <c r="T57" s="6"/>
     </row>
     <row r="58" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="4"/>
       <c r="B58" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="M58" s="6"/>
-      <c r="N58" s="6"/>
-      <c r="O58" s="6"/>
       <c r="P58" s="5"/>
-      <c r="Q58" s="6"/>
-      <c r="R58" s="6"/>
-      <c r="S58" s="6"/>
-      <c r="T58" s="6"/>
     </row>
     <row r="59" customFormat="false" ht="3.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="4"/>
@@ -1029,16 +979,16 @@
   </sheetPr>
   <dimension ref="A1:X82"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O27" activeCellId="0" sqref="O27"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B48" activeCellId="0" sqref="B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="3.88775510204082"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="33.6938775510204"/>
-    <col collapsed="false" hidden="false" max="24" min="3" style="0" width="3.88775510204082"/>
-    <col collapsed="false" hidden="false" max="1025" min="25" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="3.78061224489796"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="33.3418367346939"/>
+    <col collapsed="false" hidden="false" max="24" min="3" style="0" width="3.78061224489796"/>
+    <col collapsed="false" hidden="false" max="1025" min="25" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="21.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1418,8 +1368,6 @@
       <c r="Q34" s="5"/>
       <c r="R34" s="5"/>
       <c r="S34" s="5"/>
-      <c r="T34" s="6"/>
-      <c r="U34" s="6"/>
     </row>
     <row r="35" customFormat="false" ht="3.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="4"/>
@@ -1435,10 +1383,6 @@
       <c r="M36" s="5"/>
       <c r="N36" s="5"/>
       <c r="O36" s="5"/>
-      <c r="P36" s="6"/>
-      <c r="Q36" s="6"/>
-      <c r="R36" s="6"/>
-      <c r="S36" s="6"/>
     </row>
     <row r="37" customFormat="false" ht="3.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="4"/>
@@ -1511,6 +1455,11 @@
       <c r="M48" s="5"/>
       <c r="N48" s="5"/>
       <c r="O48" s="5"/>
+      <c r="P48" s="5"/>
+      <c r="Q48" s="5"/>
+      <c r="R48" s="5"/>
+      <c r="S48" s="5"/>
+      <c r="T48" s="5"/>
     </row>
     <row r="49" customFormat="false" ht="3.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="4"/>
@@ -1523,11 +1472,6 @@
       <c r="M50" s="5"/>
       <c r="N50" s="5"/>
       <c r="O50" s="5"/>
-      <c r="P50" s="5"/>
-      <c r="Q50" s="5"/>
-      <c r="R50" s="5"/>
-      <c r="S50" s="5"/>
-      <c r="T50" s="5"/>
     </row>
     <row r="51" customFormat="false" ht="3.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="4"/>
@@ -1546,78 +1490,37 @@
     </row>
     <row r="53" customFormat="false" ht="3.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="4"/>
-      <c r="O53" s="6"/>
-      <c r="P53" s="6"/>
-      <c r="Q53" s="6"/>
-      <c r="R53" s="6"/>
-      <c r="S53" s="6"/>
-      <c r="T53" s="6"/>
-      <c r="U53" s="6"/>
-      <c r="V53" s="6"/>
     </row>
     <row r="54" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="4"/>
       <c r="B54" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="O54" s="6"/>
-      <c r="P54" s="6"/>
+      <c r="P54" s="5"/>
       <c r="Q54" s="5"/>
-      <c r="R54" s="6"/>
-      <c r="S54" s="6"/>
-      <c r="T54" s="6"/>
-      <c r="U54" s="6"/>
-      <c r="V54" s="6"/>
+      <c r="R54" s="5"/>
+      <c r="S54" s="5"/>
+      <c r="T54" s="5"/>
     </row>
     <row r="55" customFormat="false" ht="3.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="4"/>
-      <c r="O55" s="6"/>
-      <c r="P55" s="6"/>
-      <c r="Q55" s="6"/>
-      <c r="R55" s="6"/>
-      <c r="S55" s="6"/>
-      <c r="T55" s="6"/>
-      <c r="U55" s="6"/>
-      <c r="V55" s="6"/>
     </row>
     <row r="56" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="4"/>
       <c r="B56" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="O56" s="6"/>
-      <c r="P56" s="5"/>
       <c r="Q56" s="5"/>
-      <c r="R56" s="5"/>
-      <c r="S56" s="5"/>
-      <c r="T56" s="5"/>
-      <c r="U56" s="6"/>
-      <c r="V56" s="6"/>
     </row>
     <row r="57" customFormat="false" ht="3.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="4"/>
-      <c r="O57" s="6"/>
-      <c r="P57" s="6"/>
-      <c r="Q57" s="6"/>
-      <c r="R57" s="6"/>
-      <c r="S57" s="6"/>
-      <c r="T57" s="6"/>
-      <c r="U57" s="6"/>
-      <c r="V57" s="6"/>
     </row>
     <row r="58" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="4"/>
       <c r="B58" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="O58" s="6"/>
-      <c r="P58" s="6"/>
-      <c r="Q58" s="6"/>
       <c r="R58" s="5"/>
-      <c r="S58" s="6"/>
-      <c r="T58" s="6"/>
-      <c r="U58" s="6"/>
-      <c r="V58" s="6"/>
     </row>
     <row r="59" customFormat="false" ht="3.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="4"/>
@@ -1693,7 +1596,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="8" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="8" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>

</xml_diff>